<commit_message>
Fixing bugs in MySQLDatastore automigration
</commit_message>
<xml_diff>
--- a/config/form_config/form.xlsx
+++ b/config/form_config/form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avenugopal/Desktop/UB Work/RA Project/webapp/config/form_config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avenugopal/Desktop/UB Work/RA Project/dynamic_webform/config/form_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A83FD4-AE81-E340-8759-8864651E1758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9D4D81-3B34-9345-8EAB-B60B9C4B93E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3320" yWindow="920" windowWidth="26760" windowHeight="17120" activeTab="1" xr2:uid="{49885246-638E-914D-A12E-98634A8D9864}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>select</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>Avg Yearly Income</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>Company Title</t>
   </si>
 </sst>
 </file>
@@ -215,9 +221,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -640,10 +649,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4306E8B5-6EFB-FC48-B41D-7EAB9AF1DD02}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -682,57 +691,58 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>37</v>
       </c>
-      <c r="F3" t="s">
-        <v>35</v>
-      </c>
       <c r="G3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -741,56 +751,53 @@
         <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
         <v>37</v>
       </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
       <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>37</v>
       </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
       <c r="G6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -798,21 +805,47 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
         <v>37</v>
       </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
       <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Syncing web form file
</commit_message>
<xml_diff>
--- a/config/form_config/form.xlsx
+++ b/config/form_config/form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avenugopal/Desktop/UB Work/RA Project/dynamic_webform/config/form_config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avenugopal/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9D4D81-3B34-9345-8EAB-B60B9C4B93E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8761571D-BB61-A14A-805C-7BEFB0DE9D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3320" yWindow="920" windowWidth="26760" windowHeight="17120" activeTab="1" xr2:uid="{49885246-638E-914D-A12E-98634A8D9864}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>select</t>
   </si>
@@ -87,12 +87,6 @@
     <t>Company Type</t>
   </si>
   <si>
-    <t>d-u-n-s_number</t>
-  </si>
-  <si>
-    <t>D-U-N-S@ Number</t>
-  </si>
-  <si>
     <t>import_export</t>
   </si>
   <si>
@@ -159,10 +153,19 @@
     <t>Avg Yearly Income</t>
   </si>
   <si>
-    <t>company</t>
-  </si>
-  <si>
-    <t>Company Title</t>
+    <t>new_field_2</t>
+  </si>
+  <si>
+    <t>This is a new field</t>
+  </si>
+  <si>
+    <t>Option 1, Option 2</t>
+  </si>
+  <si>
+    <t>new_field_3</t>
+  </si>
+  <si>
+    <t>Label 2</t>
   </si>
 </sst>
 </file>
@@ -221,12 +224,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -592,10 +592,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -603,10 +603,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -614,10 +614,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -625,10 +625,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -636,10 +636,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -652,13 +652,13 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" customWidth="1"/>
     <col min="6" max="6" width="68.1640625" bestFit="1" customWidth="1"/>
@@ -678,7 +678,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
@@ -691,136 +691,138 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G5">
         <v>3</v>
       </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G6">
         <v>4</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G7">
         <v>5</v>
@@ -831,19 +833,19 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G8">
         <v>1</v>

</xml_diff>